<commit_message>
Adapted the script so that data is saved in BIDS-compatible manner. - Creation of a directory for each participant. EEG data is saved in an "eeg" directory in the current participant's directory.
</commit_message>
<xml_diff>
--- a/TriggerCoding_SummaryJuly2022.xlsx
+++ b/TriggerCoding_SummaryJuly2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bolger/PycharmProjects/Syntax_SpatioTempDyn_31-05-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA86267-08D2-7043-876E-9C61EBDBB3DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6648F5-16D1-094C-B72C-2B074FA62AC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="1160" windowWidth="26440" windowHeight="15440" xr2:uid="{55183A8E-A724-684F-AE6E-9441238BDEA4}"/>
   </bookViews>
@@ -790,11 +790,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1546,7 +1546,7 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C21">
@@ -2659,7 +2659,7 @@
       <c r="A74" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C74">
@@ -2680,7 +2680,7 @@
       <c r="A75" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C75">
@@ -2701,7 +2701,7 @@
       <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C76">
@@ -2722,7 +2722,7 @@
       <c r="A77" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C77">
@@ -2743,7 +2743,7 @@
       <c r="A78" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C78">
@@ -2764,7 +2764,7 @@
       <c r="A79" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C79">
@@ -2785,7 +2785,7 @@
       <c r="A80" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C80">
@@ -2806,7 +2806,7 @@
       <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C81">
@@ -2827,7 +2827,7 @@
       <c r="A82" t="s">
         <v>8</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C82">
@@ -2848,7 +2848,7 @@
       <c r="A83" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C83">
@@ -2869,7 +2869,7 @@
       <c r="A84" t="s">
         <v>10</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C84">
@@ -2890,7 +2890,7 @@
       <c r="A85" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C85">
@@ -2911,7 +2911,7 @@
       <c r="A86" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C86">
@@ -2932,7 +2932,7 @@
       <c r="A87" t="s">
         <v>13</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C87">
@@ -2953,7 +2953,7 @@
       <c r="A88" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C88">
@@ -2974,7 +2974,7 @@
       <c r="A89" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C89">
@@ -2995,7 +2995,7 @@
       <c r="A90" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C90">
@@ -3016,7 +3016,7 @@
       <c r="A91" t="s">
         <v>17</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C91">
@@ -3037,7 +3037,7 @@
       <c r="A92" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C92">
@@ -3058,7 +3058,7 @@
       <c r="A93" t="s">
         <v>19</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>182</v>
       </c>
       <c r="C93">
@@ -3079,7 +3079,7 @@
       <c r="A94" t="s">
         <v>20</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C94">
@@ -3100,7 +3100,7 @@
       <c r="A95" t="s">
         <v>21</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C95">
@@ -3121,7 +3121,7 @@
       <c r="A96" t="s">
         <v>22</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>185</v>
       </c>
       <c r="C96">
@@ -3142,7 +3142,7 @@
       <c r="A97" t="s">
         <v>23</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C97">
@@ -3163,7 +3163,7 @@
       <c r="A98" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C98">
@@ -3184,7 +3184,7 @@
       <c r="A99" t="s">
         <v>25</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C99">
@@ -3205,7 +3205,7 @@
       <c r="A100" t="s">
         <v>26</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C100">
@@ -3226,7 +3226,7 @@
       <c r="A101" t="s">
         <v>27</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C101">
@@ -3247,7 +3247,7 @@
       <c r="A102" t="s">
         <v>28</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C102">
@@ -3268,7 +3268,7 @@
       <c r="A103" t="s">
         <v>29</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C103">
@@ -3289,7 +3289,7 @@
       <c r="A104" t="s">
         <v>30</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C104">
@@ -3310,7 +3310,7 @@
       <c r="A105" t="s">
         <v>31</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C105">
@@ -3331,7 +3331,7 @@
       <c r="A106" t="s">
         <v>32</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C106">
@@ -3352,7 +3352,7 @@
       <c r="A107" t="s">
         <v>33</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C107">
@@ -3373,7 +3373,7 @@
       <c r="A108" t="s">
         <v>34</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C108">
@@ -3394,7 +3394,7 @@
       <c r="A109" t="s">
         <v>35</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C109">
@@ -3415,7 +3415,7 @@
       <c r="A110" t="s">
         <v>36</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C110">
@@ -3436,7 +3436,7 @@
       <c r="A111" t="s">
         <v>37</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C111">
@@ -3457,7 +3457,7 @@
       <c r="A112" t="s">
         <v>38</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C112">
@@ -3478,7 +3478,7 @@
       <c r="A113" t="s">
         <v>39</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C113">
@@ -3499,7 +3499,7 @@
       <c r="A114" t="s">
         <v>40</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C114">
@@ -3520,7 +3520,7 @@
       <c r="A115" t="s">
         <v>41</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C115">
@@ -3541,7 +3541,7 @@
       <c r="A116" t="s">
         <v>42</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="2" t="s">
         <v>205</v>
       </c>
       <c r="C116">
@@ -3562,7 +3562,7 @@
       <c r="A117" t="s">
         <v>43</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C117">
@@ -3583,7 +3583,7 @@
       <c r="A118" t="s">
         <v>44</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="2" t="s">
         <v>207</v>
       </c>
       <c r="C118">
@@ -3604,7 +3604,7 @@
       <c r="A119" t="s">
         <v>45</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="2" t="s">
         <v>208</v>
       </c>
       <c r="C119">
@@ -3625,7 +3625,7 @@
       <c r="A120" t="s">
         <v>46</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>209</v>
       </c>
       <c r="C120">
@@ -3646,7 +3646,7 @@
       <c r="A121" t="s">
         <v>47</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>210</v>
       </c>
       <c r="C121">
@@ -3667,7 +3667,7 @@
       <c r="A122" t="s">
         <v>48</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="2" t="s">
         <v>211</v>
       </c>
       <c r="C122">
@@ -3688,7 +3688,7 @@
       <c r="A123" t="s">
         <v>49</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="2" t="s">
         <v>212</v>
       </c>
       <c r="C123">
@@ -3709,7 +3709,7 @@
       <c r="A124" t="s">
         <v>50</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="2" t="s">
         <v>213</v>
       </c>
       <c r="C124">
@@ -3730,7 +3730,7 @@
       <c r="A125" t="s">
         <v>51</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C125">
@@ -3751,7 +3751,7 @@
       <c r="A126" t="s">
         <v>52</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="2" t="s">
         <v>215</v>
       </c>
       <c r="C126">
@@ -3772,7 +3772,7 @@
       <c r="A127" t="s">
         <v>53</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="2" t="s">
         <v>216</v>
       </c>
       <c r="C127">
@@ -3793,7 +3793,7 @@
       <c r="A128" t="s">
         <v>54</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="2" t="s">
         <v>217</v>
       </c>
       <c r="C128">
@@ -3814,7 +3814,7 @@
       <c r="A129" t="s">
         <v>55</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C129">
@@ -3835,7 +3835,7 @@
       <c r="A130" t="s">
         <v>56</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B130" s="2" t="s">
         <v>219</v>
       </c>
       <c r="C130">
@@ -3856,14 +3856,14 @@
       <c r="A131" t="s">
         <v>57</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B131" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C131">
         <v>157</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="C131:D145" si="2">IF(C131&gt;200,1,0)</f>
+        <f t="shared" ref="D131:D144" si="2">IF(C131&gt;200,1,0)</f>
         <v>0</v>
       </c>
       <c r="E131" t="s">
@@ -3877,7 +3877,7 @@
       <c r="A132" t="s">
         <v>58</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="2" t="s">
         <v>221</v>
       </c>
       <c r="C132">
@@ -3898,7 +3898,7 @@
       <c r="A133" t="s">
         <v>59</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B133" s="2" t="s">
         <v>222</v>
       </c>
       <c r="C133">
@@ -3919,7 +3919,7 @@
       <c r="A134" t="s">
         <v>60</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B134" s="2" t="s">
         <v>223</v>
       </c>
       <c r="C134">
@@ -3940,7 +3940,7 @@
       <c r="A135" t="s">
         <v>61</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B135" s="2" t="s">
         <v>224</v>
       </c>
       <c r="C135">
@@ -3961,7 +3961,7 @@
       <c r="A136" t="s">
         <v>62</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B136" s="2" t="s">
         <v>225</v>
       </c>
       <c r="C136">
@@ -3982,7 +3982,7 @@
       <c r="A137" t="s">
         <v>63</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C137">
@@ -4003,7 +4003,7 @@
       <c r="A138" t="s">
         <v>64</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B138" s="2" t="s">
         <v>227</v>
       </c>
       <c r="C138">
@@ -4024,7 +4024,7 @@
       <c r="A139" t="s">
         <v>65</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C139">
@@ -4045,7 +4045,7 @@
       <c r="A140" t="s">
         <v>66</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B140" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C140">
@@ -4066,7 +4066,7 @@
       <c r="A141" t="s">
         <v>67</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B141" s="2" t="s">
         <v>230</v>
       </c>
       <c r="C141">
@@ -4087,7 +4087,7 @@
       <c r="A142" t="s">
         <v>68</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="B142" s="2" t="s">
         <v>231</v>
       </c>
       <c r="C142">
@@ -4108,7 +4108,7 @@
       <c r="A143" t="s">
         <v>69</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B143" s="2" t="s">
         <v>232</v>
       </c>
       <c r="C143">
@@ -4129,7 +4129,7 @@
       <c r="A144" t="s">
         <v>70</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" s="2" t="s">
         <v>233</v>
       </c>
       <c r="C144">
@@ -4150,7 +4150,7 @@
       <c r="A145" t="s">
         <v>71</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B145" s="2" t="s">
         <v>234</v>
       </c>
       <c r="C145" t="e">

</xml_diff>